<commit_message>
created a shark_geo csv file of df with go data
</commit_message>
<xml_diff>
--- a/Resource/WAProjectGrids.xlsx
+++ b/Resource/WAProjectGrids.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathe\Documents\Bootcamp\Project_Shark\Resource\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4005D3E8-0D4E-4BA3-81ED-1851AFD9A6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="17985" windowHeight="12345"/>
+    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WA Project Grids" sheetId="1" r:id="rId1"/>
@@ -787,7 +793,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000000"/>
@@ -946,6 +952,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -967,7 +976,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="Text Box 2"/>
+        <xdr:cNvPr id="1026" name="Text Box 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1036,7 +1051,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1093,7 +1114,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1168,7 +1195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1201,9 +1228,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1236,6 +1280,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1411,51 +1472,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="20" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:19" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:19" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>0</v>
       </c>
@@ -1514,7 +1575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
@@ -1571,7 +1632,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>17</v>
       </c>
@@ -1628,7 +1689,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>215</v>
       </c>
@@ -1685,7 +1746,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>24</v>
       </c>
@@ -1740,7 +1801,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>216</v>
       </c>
@@ -1795,7 +1856,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>32</v>
       </c>
@@ -1850,7 +1911,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
@@ -1907,7 +1968,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>220</v>
       </c>
@@ -1964,7 +2025,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -2021,7 +2082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>49</v>
       </c>
@@ -2078,7 +2139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>222</v>
       </c>
@@ -2135,7 +2196,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>212</v>
       </c>
@@ -2190,7 +2251,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>57</v>
       </c>
@@ -2245,7 +2306,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>223</v>
       </c>
@@ -2300,7 +2361,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>59</v>
       </c>
@@ -2357,7 +2418,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>67</v>
       </c>
@@ -2414,7 +2475,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>225</v>
       </c>
@@ -2471,7 +2532,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>69</v>
       </c>
@@ -2526,7 +2587,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>76</v>
       </c>
@@ -2581,7 +2642,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>227</v>
       </c>
@@ -2636,7 +2697,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>78</v>
       </c>
@@ -2695,7 +2756,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>229</v>
       </c>
@@ -2754,7 +2815,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>85</v>
       </c>
@@ -2809,7 +2870,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>91</v>
       </c>
@@ -2864,7 +2925,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>231</v>
       </c>
@@ -2919,7 +2980,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>96</v>
       </c>
@@ -2976,7 +3037,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>103</v>
       </c>
@@ -3033,7 +3094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>233</v>
       </c>
@@ -3090,7 +3151,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>105</v>
       </c>
@@ -3147,7 +3208,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>112</v>
       </c>
@@ -3204,7 +3265,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>235</v>
       </c>
@@ -3261,7 +3322,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>117</v>
       </c>
@@ -3316,7 +3377,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>124</v>
       </c>
@@ -3371,7 +3432,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>237</v>
       </c>
@@ -3426,7 +3487,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>129</v>
       </c>
@@ -3483,7 +3544,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>136</v>
       </c>
@@ -3540,7 +3601,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>239</v>
       </c>
@@ -3597,7 +3658,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>138</v>
       </c>
@@ -3652,7 +3713,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
         <v>240</v>
       </c>
@@ -3707,7 +3768,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>144</v>
       </c>
@@ -3762,7 +3823,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>151</v>
       </c>
@@ -3817,7 +3878,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>242</v>
       </c>
@@ -3872,7 +3933,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>153</v>
       </c>
@@ -3929,7 +3990,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>159</v>
       </c>
@@ -3986,7 +4047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>244</v>
       </c>
@@ -4043,7 +4104,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>161</v>
       </c>
@@ -4100,7 +4161,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>168</v>
       </c>
@@ -4157,7 +4218,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>246</v>
       </c>
@@ -4214,7 +4275,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>170</v>
       </c>
@@ -4271,7 +4332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>177</v>
       </c>
@@ -4328,7 +4389,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
         <v>248</v>
       </c>
@@ -4385,7 +4446,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>180</v>
       </c>
@@ -4442,7 +4503,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>187</v>
       </c>
@@ -4499,7 +4560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
         <v>250</v>
       </c>
@@ -4556,7 +4617,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>190</v>
       </c>
@@ -4611,7 +4672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>197</v>
       </c>
@@ -4666,7 +4727,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
         <v>252</v>
       </c>

</xml_diff>